<commit_message>
updated library selection scripts with correct global. resolved some issues. passing on to Yizhen for "" \\ issue.
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_CDS_Filter_LibrarySelection-HybridSelection.xlsx
+++ b/InputFiles/TC01_CDS_Filter_LibrarySelection-HybridSelection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\podagatlapalll2\CDS Automation\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\prasanna\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26893123-3312-42EF-B3CD-83EA5B9603EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7801A55-EEFB-437D-8973-1AB77AA9EF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -494,12 +494,12 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="52" zoomScaleNormal="52" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="96.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="74.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="78.90625" style="1" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
fix from Yizhen for \\omic\\ in cds corrected test cases in library selection cds
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_CDS_Filter_LibrarySelection-HybridSelection.xlsx
+++ b/InputFiles/TC01_CDS_Filter_LibrarySelection-HybridSelection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\prasanna\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7801A55-EEFB-437D-8973-1AB77AA9EF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B86D29-693A-404B-8394-2E1E0AEFF9D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -54,19 +54,6 @@
     <t>FilesTab</t>
   </si>
   <si>
-    <t>Match (f)&lt;--(g:genomic_info)
-WHERE g.library_selection in ['Hybrid Selection']
-MATCH (f)--&gt;(samp:sample)--&gt;(p:participant)--&gt;(s:study)
-WITH p, s, collect(distinct samp.sample_id) as samp
-RETURN 
-coalesce(p.participant_id,'') as `Participant ID`,
-coalesce(s.study_name, '') as `Study Name`,
-coalesce(s.phs_accession,'') as `Accession`,
-coalesce(p.gender,'') as `Gender`,
-coalesce(apoc.text.join(samp, ','), '') as `Samples`
-ORDER BY `Participant ID`LIMIT 100</t>
-  </si>
-  <si>
     <t>MATCH (f:file)
 Match (f)&lt;--(g:genomic_info)
 WHERE g.library_selection in ['Hybrid Selection']
@@ -114,6 +101,19 @@
   </si>
   <si>
     <t>ParticipantsTab</t>
+  </si>
+  <si>
+    <t>Match (f)&lt;--(g:genomic_info)
+WHERE g.library_selection in ['Hybrid Selection']
+MATCH (f)--&gt;(samp:sample)--&gt;(p:participant)--&gt;(s:study)
+WITH p, s, apoc.coll.sort(collect(distinct(samp.sample_id))) as samples
+RETURN 
+coalesce(p.participant_id,'') as `Participant ID`,
+coalesce(s.study_name, '') as `Study Name`,
+coalesce(s.phs_accession,'') as `Accession`,
+coalesce(p.gender,'') as `Gender`,
+coalesce(apoc.text.join(samples, ','), '') as `Samples`
+ORDER BY `Participant ID`LIMIT 100</t>
   </si>
 </sst>
 </file>
@@ -494,20 +494,20 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="52" zoomScaleNormal="52" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="96.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="74.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="77.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.08984375" style="1"/>
+    <col min="1" max="1" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="96.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="77.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -524,62 +524,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="242.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="382.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="260.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="260.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="4" spans="1:5" ht="279.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" ht="279.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C6" s="2"/>
     </row>
   </sheetData>

</xml_diff>